<commit_message>
Routing handling for armies
</commit_message>
<xml_diff>
--- a/battles/Hydaspes/Hydaspes.xlsx
+++ b/battles/Hydaspes/Hydaspes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\training\gboh-companion\battles\Hydaspes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97CBC32-73C8-40D4-BA94-03C4CFA3A087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CA42C2-4B39-4DD1-A003-B3C3C42E2621}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indian" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="136">
   <si>
     <t>Kind</t>
   </si>
@@ -431,6 +431,24 @@
   </si>
   <si>
     <t>LI16</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>Bactrian</t>
+  </si>
+  <si>
+    <t>Arachosian</t>
+  </si>
+  <si>
+    <t>Parapamasidian</t>
+  </si>
+  <si>
+    <t>MJ</t>
+  </si>
+  <si>
+    <t>MA</t>
   </si>
 </sst>
 </file>
@@ -1363,8 +1381,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D87D165A-15F5-4328-ACD3-D3D33A98CD06}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A31:B49" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D87D165A-15F5-4328-ACD3-D3D33A98CD06}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A35:B53" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
       <items count="9">
@@ -1477,8 +1495,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64CD77FD-45F6-487F-9339-BEB42CFD4DEB}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="N31:O37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64CD77FD-45F6-487F-9339-BEB42CFD4DEB}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="N35:O41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1869,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:M60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="A1:M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3517,10 +3535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="A1:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4047,7 +4065,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -4069,7 +4087,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="10"/>
@@ -4080,7 +4098,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4102,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="10"/>
@@ -4113,7 +4131,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -4134,7 +4152,7 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="10"/>
@@ -4145,7 +4163,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -4166,7 +4184,7 @@
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ref="M20" si="15">IF(OR(RIGHT(A20)="C",A20="LN"),"Cavalry",IF(OR(RIGHT(A20)="I",A20="PH",A20="LP"),"Infantry",A20))</f>
@@ -4177,7 +4195,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -4198,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="10"/>
@@ -4209,7 +4227,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -4239,7 +4257,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -4269,7 +4287,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -4299,7 +4317,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -4310,7 +4328,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f t="shared" ref="E25:E26" si="17">LEFT(C25,1)&amp;A25&amp;LEFT(D25)</f>
+        <f t="shared" ref="E25:E29" si="17">LEFT(C25,1)&amp;A25&amp;LEFT(D25)</f>
         <v>CHC3</v>
       </c>
       <c r="F25" s="1">
@@ -4321,15 +4339,15 @@
       </c>
       <c r="H25" s="1"/>
       <c r="M25" t="str">
-        <f t="shared" ref="M25:M26" si="18">IF(OR(RIGHT(A25)="C",A25="LN"),"Cavalry",IF(OR(RIGHT(A25)="I",A25="PH",A25="LP"),"Infantry",A25))</f>
+        <f t="shared" ref="M25:M29" si="18">IF(OR(RIGHT(A25)="C",A25="LN"),"Cavalry",IF(OR(RIGHT(A25)="I",A25="PH",A25="LP"),"Infantry",A25))</f>
         <v>Cavalry</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N26" si="19">IF(M25="Cavalry",G25*100,IF(M25="Infantry",G25*150,0))</f>
+        <f t="shared" ref="N25:N29" si="19">IF(M25="Cavalry",G25*100,IF(M25="Infantry",G25*150,0))</f>
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -4359,212 +4377,345 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>BHC1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>7</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="18"/>
+        <v>Cavalry</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="19"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>ALC1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>7</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>134</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="18"/>
+        <v>Cavalry</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="19"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>PLC1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>134</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="18"/>
+        <v>Cavalry</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="19"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" ref="E30" si="20">LEFT(C30,1)&amp;A30&amp;LEFT(D30)</f>
+        <v>CHC5</v>
+      </c>
+      <c r="F30" s="1">
+        <v>8</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="M30" t="str">
+        <f t="shared" ref="M30" si="21">IF(OR(RIGHT(A30)="C",A30="LN"),"Cavalry",IF(OR(RIGHT(A30)="I",A30="PH",A30="LP"),"Infantry",A30))</f>
+        <v>Cavalry</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ref="N30" si="22">IF(M30="Cavalry",G30*100,IF(M30="Infantry",G30*150,0))</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="F28">
-        <f>SUM(F2:F26)</f>
-        <v>163</v>
-      </c>
-      <c r="G28">
-        <f>SUM(G2:G26)</f>
-        <v>132</v>
-      </c>
-      <c r="N28">
-        <f>SUM(N2:N26)</f>
-        <v>16650</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="F32">
+        <f>SUM(F2:F29)</f>
+        <v>184</v>
+      </c>
+      <c r="G32">
+        <f>SUM(G2:G29)</f>
+        <v>142</v>
+      </c>
+      <c r="N32">
+        <f>SUM(N2:N29)</f>
+        <v>17650</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="N36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="4">
+      <c r="O36" s="4">
         <v>3800</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>8</v>
-      </c>
-      <c r="B33" s="4">
-        <v>2</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O33" s="4">
-        <v>11850</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>9</v>
-      </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="4">
-        <v>3</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>8</v>
-      </c>
-      <c r="B36" s="4">
-        <v>2</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
+        <v>8</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O37" s="4">
+        <v>11850</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>9</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B38" s="4">
         <v>1</v>
       </c>
-      <c r="N37" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O37" s="4">
-        <v>15650</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="4">
-        <v>5</v>
+      <c r="N38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>5</v>
+      <c r="A39" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B39" s="4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B40" s="4">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" s="4"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>17</v>
+      <c r="A41" s="5">
+        <v>9</v>
       </c>
       <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O41" s="4">
+        <v>15650</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>5</v>
+      </c>
+      <c r="B43" s="4">
         <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>5</v>
-      </c>
-      <c r="B42" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="4">
-        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B46" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B47" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B48" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>4</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>6</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B53" s="4">
         <v>23</v>
       </c>
     </row>

</xml_diff>